<commit_message>
Finished test scenario 02
</commit_message>
<xml_diff>
--- a/scenario.xlsx
+++ b/scenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ewa\Documents\__Programowanie2019\testy\JuiceShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F315D-18DA-4B32-BA98-D42EC948DA78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6212C964-2A5F-4123-B272-4E13D01183B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9615" xr2:uid="{23FA8D9F-820A-4813-B253-167303C2F70D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Test Scenario #</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Check the system behavior when email adress is blank</t>
   </si>
 </sst>
 </file>
@@ -324,7 +327,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
@@ -349,6 +352,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +382,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -697,17 +712,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927411B8-7AF0-432D-B167-6560A62E4D4C}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3.7109375" style="18" customWidth="1"/>
+    <col min="3" max="4" width="3.7109375" style="19" customWidth="1"/>
     <col min="5" max="5" width="93" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" customWidth="1"/>
@@ -716,11 +731,11 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
@@ -729,8 +744,8 @@
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
@@ -741,14 +756,14 @@
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -768,7 +783,7 @@
       <c r="E5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="22" t="s">
         <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -776,8 +791,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3">
@@ -789,14 +804,14 @@
       <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="22" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="3">
         <v>3</v>
       </c>
@@ -806,14 +821,14 @@
       <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="3">
         <v>4</v>
       </c>
@@ -823,14 +838,14 @@
       <c r="E8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>37</v>
       </c>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3">
         <v>5</v>
       </c>
@@ -840,14 +855,14 @@
       <c r="E9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="3">
         <v>6</v>
       </c>
@@ -857,7 +872,9 @@
       <c r="E10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -872,7 +889,9 @@
       <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,143 +907,159 @@
       <c r="D12" s="3">
         <v>0</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="10">
+      <c r="F13" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="10">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="3">
+      <c r="E16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="3">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="3">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3">
         <v>2</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="3">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="3">
         <v>3</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>3</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="3">
-        <v>3</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8" t="s">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="19" t="s">
-        <v>5</v>
-      </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="19" t="s">
-        <v>6</v>
+      <c r="B22" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="19" t="s">
-        <v>7</v>
+      <c r="B23" s="20" t="s">
+        <v>6</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1033,8 +1068,8 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="19" t="s">
-        <v>8</v>
+      <c r="B24" s="20" t="s">
+        <v>7</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1043,8 +1078,8 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="19" t="s">
-        <v>9</v>
+      <c r="B25" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1053,8 +1088,8 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="19" t="s">
-        <v>10</v>
+      <c r="B26" s="20" t="s">
+        <v>9</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1063,8 +1098,8 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="19" t="s">
-        <v>11</v>
+      <c r="B27" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1073,8 +1108,8 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="19" t="s">
-        <v>12</v>
+      <c r="B28" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1083,7 +1118,9 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="5"/>
@@ -1113,19 +1150,27 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B13:B17"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="A12:A17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" location="/register" xr:uid="{3AB48899-25BC-43F3-9D54-71C10FC87BF3}"/>
+    <hyperlink ref="B19" r:id="rId1" location="/register" xr:uid="{3AB48899-25BC-43F3-9D54-71C10FC87BF3}"/>
     <hyperlink ref="B13" r:id="rId2" location="/forgot-password" xr:uid="{3E2C6E22-D9FC-4CB1-AAD2-50C62531640E}"/>
     <hyperlink ref="B6" r:id="rId3" location="/login" xr:uid="{A65FE58F-B69D-4A5C-B2FB-D7D5E43EDD1E}"/>
     <hyperlink ref="B2" r:id="rId4" location="/" xr:uid="{5EFC281D-DAE1-4D1E-A6AB-CCFADBE45E66}"/>

</xml_diff>